<commit_message>
Updated with multipart change
</commit_message>
<xml_diff>
--- a/rest-post/src/test/resources/rest/rest-post.xlsx
+++ b/rest-post/src/test/resources/rest/rest-post.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\december-release\microservices-lowcode-testautomation\rest-post\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8F6F75-A553-4530-9B37-5D9AC6BB8232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27253CEF-496E-44F5-879A-2DD0F25645A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Examples" sheetId="3" r:id="rId1"/>
+    <sheet name="Example-AttachFile" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -90,9 +91,6 @@
 }</t>
   </si>
   <si>
-    <t>https://live.virtualandemo.com/api/riskfactor/compute</t>
-  </si>
-  <si>
     <t>RiskFactor-DirtectResponse</t>
   </si>
   <si>
@@ -112,6 +110,39 @@
   </si>
   <si>
     <t>endpoint</t>
+  </si>
+  <si>
+    <t>idai</t>
+  </si>
+  <si>
+    <t>multipart/form-data</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/riskfactor/compute</t>
+  </si>
+  <si>
+    <t>RequestHeaders</t>
+  </si>
+  <si>
+    <t>testExecuted=true</t>
+  </si>
+  <si>
+    <t>http://microservices.virtualandemo.com:8900/test</t>
+  </si>
+  <si>
+    <t>Accept=*/*</t>
+  </si>
+  <si>
+    <t>filestream=sample.json;serverurl=https://live.virtualandemo.com/api;dataload=APITEST.json;execute=true;type=VIRTUALAN</t>
+  </si>
+  <si>
+    <t>Attach file with multipart</t>
+  </si>
+  <si>
+    <t>Attachement-Example</t>
+  </si>
+  <si>
+    <t>MultiFormParams</t>
   </si>
 </sst>
 </file>
@@ -257,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -272,6 +303,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -589,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +670,7 @@
         <v>11</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>12</v>
@@ -653,24 +685,24 @@
         <v>15</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>9</v>
@@ -688,13 +720,13 @@
         <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -703,4 +735,120 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7606762-C3E9-4662-AFD1-65E36C031EDD}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="98.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6">
+        <v>201</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B359BBAA-53E3-4808-AEB1-021233B4FFD5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>